<commit_message>
update test package and composition
</commit_message>
<xml_diff>
--- a/data/secr.composition.reshape.xlsx
+++ b/data/secr.composition.reshape.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RossTyzackPitman/Documents/OneDrive/PhD/Data/R_Database/R_PROJECTS/Survey_Reports/Camera-trapping/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RossTyzackPitman/Documents/OneDrive/PhD/Data/R_Database/R_PROJECTS/PhD_Chapter3/MSE_Paper/LEOPARD-MP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="1100" yWindow="1080" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
     <sheet name="secr.composition.reshape" sheetId="1" r:id="rId2"/>
     <sheet name="pivot" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId4"/>
+    <pivotCache cacheId="26" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -165,7 +165,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -219,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:F11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -1524,10 +1524,13 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>